<commit_message>
Case study cuoi khoa
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -883,6 +883,81 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SV017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Nguyễn Quốc Hưng</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1998</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tốt nghiệp</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SV018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Nguyễn Nghĩa</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1996</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tốt nghiệp</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SV019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Trần Hồng</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1996</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Chưa tốt nghiệp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>